<commit_message>
added dummy files in each folder
</commit_message>
<xml_diff>
--- a/ProjectMasterLocator.xlsx
+++ b/ProjectMasterLocator.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7332" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Project Master Locator</t>
   </si>
@@ -203,13 +203,6 @@
   </si>
   <si>
     <t>PO including Customer supplied documents, Kickoff, PIF, MOM, WSR, emails, coding std, All type of checklist, DP analysis, Metrics, PMS&gt;Monitoring other tabs(CAR, Issue tracker, Lesson learnt, Best practice, customer supplied item), QTS, CR Register, Test Report/Test results, DAR</t>
-  </si>
-  <si>
-    <t>Sohil Shah
-Faiyaz Pisuwala</t>
-  </si>
-  <si>
-    <t>Preeti Viramgami</t>
   </si>
   <si>
     <t>Automated Book Retrieval System</t>
@@ -1287,6 +1280,51 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1302,12 +1340,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1341,43 +1373,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1386,12 +1391,6 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1402,12 +1401,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1765,7 +1758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1867,7 +1860,7 @@
     </row>
     <row r="6" spans="1:17" s="24" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A6" s="106" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="106"/>
       <c r="C6" s="106"/>
@@ -1995,7 +1988,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="107" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" s="108"/>
       <c r="C20" s="108"/>
@@ -2632,7 +2625,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2648,44 +2641,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="138"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="120"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141" t="s">
+      <c r="C2" s="123"/>
+      <c r="D2" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141" t="s">
+      <c r="E2" s="123"/>
+      <c r="F2" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="142"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
+      <c r="G2" s="124"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
       <c r="P2" s="38"/>
       <c r="Q2" s="38"/>
       <c r="R2" s="38"/>
     </row>
     <row r="3" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="140"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="99" t="s">
         <v>9</v>
       </c>
@@ -2704,26 +2697,18 @@
       <c r="G3" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="113"/>
-      <c r="K3" s="113"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="113"/>
-      <c r="N3" s="113"/>
-      <c r="O3" s="113"/>
-    </row>
-    <row r="4" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="98" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="98">
-        <v>43056</v>
-      </c>
-      <c r="D4" s="98" t="s">
-        <v>56</v>
-      </c>
+      <c r="J3" s="128"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="128"/>
+      <c r="N3" s="128"/>
+      <c r="O3" s="128"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="98"/>
       <c r="F4" s="98"/>
       <c r="G4" s="101"/>
@@ -2777,61 +2762,61 @@
       <c r="A10" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="124" t="s">
+      <c r="B10" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="125"/>
+      <c r="C10" s="137"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
+      <c r="G10" s="138"/>
     </row>
     <row r="11" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="135"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="117"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="73"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="135"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="117"/>
     </row>
     <row r="13" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="73"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="135"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="117"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="73"/>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="135"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="117"/>
     </row>
     <row r="15" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="74"/>
-      <c r="B15" s="129"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
-      <c r="G15" s="130"/>
+      <c r="B15" s="142"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="142"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="143"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="55"/>
@@ -2852,73 +2837,73 @@
       <c r="G17" s="59"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="136" t="s">
+      <c r="A18" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="137"/>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="138"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="127"/>
-      <c r="C19" s="127" t="s">
+      <c r="B19" s="140"/>
+      <c r="C19" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="127"/>
-      <c r="E19" s="128"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="141"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="143"/>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="119"/>
+      <c r="A20" s="125"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="127"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="143"/>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="119"/>
+      <c r="A21" s="125"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="127"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="116"/>
-      <c r="B22" s="117"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="119"/>
+      <c r="A22" s="131"/>
+      <c r="B22" s="132"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="127"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="116"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="119"/>
+      <c r="A23" s="131"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="127"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="116"/>
-      <c r="B24" s="117"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="119"/>
+      <c r="A24" s="131"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="126"/>
+      <c r="E24" s="127"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="116"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="119"/>
+      <c r="A25" s="131"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="127"/>
     </row>
     <row r="26" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="120"/>
-      <c r="B26" s="121"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122"/>
-      <c r="E26" s="123"/>
+      <c r="A26" s="133"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="136"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="58"/>
@@ -2930,21 +2915,21 @@
       <c r="G27" s="58"/>
     </row>
     <row r="29" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="114"/>
-      <c r="B29" s="115"/>
-      <c r="C29" s="115"/>
-      <c r="D29" s="115"/>
-      <c r="E29" s="115"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
+      <c r="A29" s="129"/>
+      <c r="B29" s="130"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="131" t="s">
+      <c r="A30" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="132"/>
-      <c r="C30" s="132"/>
-      <c r="D30" s="133"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="115"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
@@ -3004,21 +2989,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
     <mergeCell ref="J2:O3"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A22:B22"/>
@@ -3035,6 +3005,21 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="B15:G15"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3066,11 +3051,11 @@
       <c r="B2" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="144" t="s">
+      <c r="C2" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="144"/>
-      <c r="E2" s="145"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="149"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
@@ -3086,11 +3071,11 @@
       <c r="B3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="150" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="148"/>
-      <c r="E3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
@@ -3106,11 +3091,11 @@
       <c r="B4" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="151"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="153"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
@@ -3142,11 +3127,11 @@
       <c r="B6" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="144"/>
-      <c r="E6" s="145"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="149"/>
       <c r="F6" s="33"/>
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
@@ -3162,11 +3147,11 @@
       <c r="B7" s="83">
         <v>1</v>
       </c>
-      <c r="C7" s="146" t="s">
+      <c r="C7" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="146"/>
-      <c r="E7" s="147"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="145"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
@@ -3182,11 +3167,11 @@
       <c r="B8" s="83">
         <v>2</v>
       </c>
-      <c r="C8" s="146" t="s">
+      <c r="C8" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="146"/>
-      <c r="E8" s="147"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="145"/>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
@@ -3202,11 +3187,11 @@
       <c r="B9" s="83">
         <v>3</v>
       </c>
-      <c r="C9" s="146" t="s">
+      <c r="C9" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="146"/>
-      <c r="E9" s="147"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="145"/>
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
@@ -3222,11 +3207,11 @@
       <c r="B10" s="83">
         <v>4</v>
       </c>
-      <c r="C10" s="146" t="s">
+      <c r="C10" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="146"/>
-      <c r="E10" s="147"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="145"/>
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
@@ -3242,11 +3227,11 @@
       <c r="B11" s="83">
         <v>5</v>
       </c>
-      <c r="C11" s="146" t="s">
+      <c r="C11" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="146"/>
-      <c r="E11" s="147"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="145"/>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
       <c r="H11" s="33"/>
@@ -3262,11 +3247,11 @@
       <c r="B12" s="83">
         <v>6</v>
       </c>
-      <c r="C12" s="146" t="s">
+      <c r="C12" s="144" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="146"/>
-      <c r="E12" s="147"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="145"/>
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
@@ -3282,11 +3267,11 @@
       <c r="B13" s="83">
         <v>7</v>
       </c>
-      <c r="C13" s="146" t="s">
+      <c r="C13" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="146"/>
-      <c r="E13" s="147"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="145"/>
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
       <c r="H13" s="33"/>
@@ -3302,11 +3287,11 @@
       <c r="B14" s="83">
         <v>8</v>
       </c>
-      <c r="C14" s="146" t="s">
+      <c r="C14" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="146"/>
-      <c r="E14" s="147"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="145"/>
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
@@ -3322,11 +3307,11 @@
       <c r="B15" s="83">
         <v>9</v>
       </c>
-      <c r="C15" s="146" t="s">
+      <c r="C15" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="146"/>
-      <c r="E15" s="147"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="145"/>
       <c r="F15" s="33"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
@@ -3342,11 +3327,11 @@
       <c r="B16" s="83">
         <v>10</v>
       </c>
-      <c r="C16" s="146" t="s">
+      <c r="C16" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="146"/>
-      <c r="E16" s="147"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="145"/>
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
@@ -3362,11 +3347,11 @@
       <c r="B17" s="84">
         <v>11</v>
       </c>
-      <c r="C17" s="152" t="s">
+      <c r="C17" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="152"/>
-      <c r="E17" s="153"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="147"/>
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
@@ -3469,6 +3454,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C2:E2"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
@@ -3479,11 +3469,6 @@
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3494,7 +3479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>

</xml_diff>